<commit_message>
os_concepts inside vim removed
</commit_message>
<xml_diff>
--- a/Unix Pre requisite CSGI.xlsx
+++ b/Unix Pre requisite CSGI.xlsx
@@ -15,6 +15,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">UniX!$B$1:$F$184</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">UniX!$B$1:$F$184</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">UniX!$B$1:$F$184</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">UniX!$B$1:$F$184</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
@@ -899,8 +900,8 @@
   </sheetPr>
   <dimension ref="A1:F184"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A54" activeCellId="0" sqref="A54"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A76" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A113" activeCellId="0" sqref="A113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -915,6 +916,7 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0"/>
       <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
@@ -932,6 +934,7 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0"/>
       <c r="B2" s="5" t="s">
         <v>5</v>
       </c>
@@ -947,6 +950,7 @@
       <c r="F2" s="6"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0"/>
       <c r="B3" s="5" t="s">
         <v>9</v>
       </c>
@@ -960,6 +964,7 @@
       <c r="F3" s="6"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0"/>
       <c r="B4" s="5" t="s">
         <v>10</v>
       </c>
@@ -973,6 +978,7 @@
       <c r="F4" s="6"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0"/>
       <c r="B5" s="5" t="s">
         <v>11</v>
       </c>
@@ -986,6 +992,7 @@
       <c r="F5" s="6"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0"/>
       <c r="B6" s="5" t="s">
         <v>12</v>
       </c>
@@ -999,6 +1006,7 @@
       <c r="F6" s="6"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0"/>
       <c r="B7" s="5" t="s">
         <v>13</v>
       </c>
@@ -1012,6 +1020,7 @@
       <c r="F7" s="6"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0"/>
       <c r="B8" s="5" t="s">
         <v>15</v>
       </c>
@@ -1025,6 +1034,7 @@
       <c r="F8" s="6"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0"/>
       <c r="B9" s="5" t="s">
         <v>16</v>
       </c>
@@ -1038,6 +1048,7 @@
       <c r="F9" s="6"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0"/>
       <c r="B10" s="5" t="s">
         <v>17</v>
       </c>
@@ -2213,7 +2224,7 @@
       <c r="F94" s="6"/>
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="10"/>
+      <c r="A95" s="11"/>
       <c r="B95" s="12" t="s">
         <v>102</v>
       </c>
@@ -2227,7 +2238,7 @@
       <c r="F95" s="6"/>
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="10"/>
+      <c r="A96" s="11"/>
       <c r="B96" s="12" t="s">
         <v>103</v>
       </c>
@@ -2241,7 +2252,7 @@
       <c r="F96" s="6"/>
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="10"/>
+      <c r="A97" s="11"/>
       <c r="B97" s="12" t="s">
         <v>104</v>
       </c>
@@ -2255,7 +2266,7 @@
       <c r="F97" s="6"/>
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="10"/>
+      <c r="A98" s="11"/>
       <c r="B98" s="12" t="s">
         <v>105</v>
       </c>
@@ -2283,7 +2294,7 @@
       <c r="F99" s="6"/>
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="10"/>
+      <c r="A100" s="11"/>
       <c r="B100" s="12" t="s">
         <v>107</v>
       </c>
@@ -2297,7 +2308,7 @@
       <c r="F100" s="6"/>
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="10"/>
+      <c r="A101" s="11"/>
       <c r="B101" s="12" t="s">
         <v>108</v>
       </c>
@@ -2311,7 +2322,7 @@
       <c r="F101" s="6"/>
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="10"/>
+      <c r="A102" s="11"/>
       <c r="B102" s="12" t="s">
         <v>109</v>
       </c>
@@ -2381,7 +2392,7 @@
       <c r="F106" s="6"/>
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="10"/>
+      <c r="A107" s="11"/>
       <c r="B107" s="12" t="s">
         <v>114</v>
       </c>

</xml_diff>